<commit_message>
Add IC2 addons, some Inductive Automation, start Mekanism, removed Nuclear Control
</commit_message>
<xml_diff>
--- a/bundle.json v5.xlsx
+++ b/bundle.json v5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason\AppData\Roaming\PrismLauncher\instances\Volentus FileDirector\minecraft\config\mod-director\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCB84FF2-2C9E-47F8-B6E6-2414DBDADBE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B21F213-2A07-40D1-94D8-54E0EA400B35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="839" activeTab="3" xr2:uid="{9C62C9EC-1015-4AFA-B33E-B214A55E5F8C}"/>
+    <workbookView xWindow="372" yWindow="216" windowWidth="22392" windowHeight="12024" tabRatio="839" activeTab="8" xr2:uid="{9C62C9EC-1015-4AFA-B33E-B214A55E5F8C}"/>
   </bookViews>
   <sheets>
     <sheet name="CurseForge" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1192" uniqueCount="872">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1222" uniqueCount="883">
   <si>
     <t>addonId</t>
   </si>
@@ -2659,13 +2659,46 @@
   </si>
   <si>
     <t>https://www.curseforge.com/minecraft/mc-mods/wanionlib</t>
+  </si>
+  <si>
+    <t>Technomancy - 0.12.5 - 1.7.10.jar</t>
+  </si>
+  <si>
+    <t>Technomancy</t>
+  </si>
+  <si>
+    <t>https://mediafilez.forgecdn.net/files/2295/819/Technomancy - 0.12.5 - 1.7.10.jar</t>
+  </si>
+  <si>
+    <t>Already have Energy Control</t>
+  </si>
+  <si>
+    <t>Jonius7 Fork fixes bug</t>
+  </si>
+  <si>
+    <t>Too many crashing items</t>
+  </si>
+  <si>
+    <t>Replaced by GTNH version</t>
+  </si>
+  <si>
+    <t>Replaced by Jonius7 Fork</t>
+  </si>
+  <si>
+    <t>Replaced by DrParadox7 version</t>
+  </si>
+  <si>
+    <t>Disabled</t>
+  </si>
+  <si>
+    <t>Not needed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2690,6 +2723,13 @@
       <u/>
       <sz val="8"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2733,7 +2773,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -2745,6 +2785,17 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
       <bottom style="thin">
         <color theme="1"/>
       </bottom>
@@ -2774,21 +2825,29 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="27">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6565"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -2904,6 +2963,23 @@
     </dxf>
     <dxf>
       <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6565"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <fill>
         <patternFill patternType="solid">
           <fgColor theme="0" tint="-0.14999847407452621"/>
           <bgColor theme="0" tint="-0.14999847407452621"/>
@@ -2945,6 +3021,9 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -3001,7 +3080,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CF71CB59-A681-467E-A496-DF22C8F63C36}" name="Table1" displayName="Table1" ref="A1:M155" totalsRowShown="0" headerRowDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CF71CB59-A681-467E-A496-DF22C8F63C36}" name="Table1" displayName="Table1" ref="A1:M155" totalsRowShown="0" headerRowDxfId="26">
   <autoFilter ref="A1:M155" xr:uid="{CF71CB59-A681-467E-A496-DF22C8F63C36}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L80">
     <sortCondition ref="E1:E80"/>
@@ -3037,7 +3116,7 @@
     <tableColumn id="8" xr3:uid="{071FB076-79DA-4271-9B11-D3DAF5A27A08}" name="selectedByDefault"/>
     <tableColumn id="9" xr3:uid="{3CDEFED8-BDC9-47C7-831C-532778102D77}" name="description"/>
     <tableColumn id="1" xr3:uid="{E6FB84AB-CA8F-4CC7-B1A7-BC7A68F80D0F}" name="name"/>
-    <tableColumn id="2" xr3:uid="{F0A7EA2F-C2AC-43F5-BC6D-C49D0647EFC8}" name="url" dataDxfId="21" dataCellStyle="Hyperlink"/>
+    <tableColumn id="2" xr3:uid="{F0A7EA2F-C2AC-43F5-BC6D-C49D0647EFC8}" name="url" dataDxfId="25" dataCellStyle="Hyperlink"/>
     <tableColumn id="6" xr3:uid="{EC64C9C3-AEEF-4EBD-8BFF-4E2922D06865}" name="side"/>
     <tableColumn id="4" xr3:uid="{9F48CDE4-D924-41EA-B9F4-C5D89CD73B03}" name="fileName"/>
     <tableColumn id="5" xr3:uid="{7F05F574-DA53-49C9-8050-3D2CCDAB677A}" name="follows"/>
@@ -3045,7 +3124,7 @@
     <tableColumn id="11" xr3:uid="{D819B850-F57B-498C-825C-8A486975641F}" name="Notes"/>
     <tableColumn id="12" xr3:uid="{49D1682B-534D-4059-A5DA-B3CA78E5F4FB}" name="folder"/>
     <tableColumn id="13" xr3:uid="{4E3663E0-B283-45F0-9C3F-F05498D5CFFD}" name="Repo" dataCellStyle="Hyperlink"/>
-    <tableColumn id="14" xr3:uid="{D8C83F8D-C674-4041-9191-44B2463F4BF7}" name="sourceFileName" dataDxfId="1">
+    <tableColumn id="14" xr3:uid="{D8C83F8D-C674-4041-9191-44B2463F4BF7}" name="sourceFileName" dataDxfId="24">
       <calculatedColumnFormula>IF(H2&lt;&gt;"", H2, RIGHT(F2,LEN(F2)-FIND("@",SUBSTITUTE(F2,"/","@",LEN(F2)-LEN(SUBSTITUTE(F2,"/",""))))))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="15" xr3:uid="{AC8070E0-756B-431E-A1EC-4CB67F73C9E2}" name="followsIL"/>
@@ -3055,7 +3134,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{837A1DAE-8158-4E48-816C-7B02D8E95473}" name="Table6" displayName="Table6" ref="A1:M28" totalsRowShown="0" headerRowDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{837A1DAE-8158-4E48-816C-7B02D8E95473}" name="Table6" displayName="Table6" ref="A1:M28" totalsRowShown="0" headerRowDxfId="23">
   <autoFilter ref="A1:M28" xr:uid="{837A1DAE-8158-4E48-816C-7B02D8E95473}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L28">
     <sortCondition ref="E1:E28"/>
@@ -3084,17 +3163,17 @@
   <autoFilter ref="E1:N13" xr:uid="{8FA21BC5-EE0E-4191-BC63-9EB4198DCDF8}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{60D5533B-280C-4133-820D-E94C6E9E36DB}" name="name"/>
-    <tableColumn id="2" xr3:uid="{66EF7A2B-9A21-4085-93F7-14CD58F6F15B}" name="url" dataDxfId="19" dataCellStyle="Hyperlink"/>
+    <tableColumn id="2" xr3:uid="{66EF7A2B-9A21-4085-93F7-14CD58F6F15B}" name="url" dataDxfId="22" dataCellStyle="Hyperlink"/>
     <tableColumn id="3" xr3:uid="{C0731F1D-4A65-4CA3-9F35-0689AF888300}" name="side"/>
     <tableColumn id="4" xr3:uid="{20970281-086F-4DD1-BF01-7E06711A2DDF}" name="fileName"/>
     <tableColumn id="5" xr3:uid="{B177552A-E452-47D5-80D6-29CB46C2F510}" name="follows"/>
     <tableColumn id="6" xr3:uid="{1962D553-6A3F-4CA6-927C-7A94E4C9757F}" name="License"/>
     <tableColumn id="7" xr3:uid="{48F547D9-B9D6-48B9-BAA7-B1972742C050}" name="Notes"/>
     <tableColumn id="8" xr3:uid="{948716AE-E46C-40AC-A5A6-5231FDD8884A}" name="folder"/>
-    <tableColumn id="9" xr3:uid="{4F45D914-640E-4DCB-A55E-32DFDD6BE6BC}" name="Repo" dataDxfId="18" dataCellStyle="Hyperlink">
+    <tableColumn id="9" xr3:uid="{4F45D914-640E-4DCB-A55E-32DFDD6BE6BC}" name="Repo" dataDxfId="21" dataCellStyle="Hyperlink">
       <calculatedColumnFormula>LEFT(F2, FIND("/releases", F2) - 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{82D64721-6A58-4E8F-B4CC-4E9A79C19880}" name="sourceFileName" dataDxfId="0">
+    <tableColumn id="10" xr3:uid="{82D64721-6A58-4E8F-B4CC-4E9A79C19880}" name="sourceFileName" dataDxfId="20">
       <calculatedColumnFormula>IF(H2&lt;&gt;"", H2, RIGHT(F2,LEN(F2)-FIND("@",SUBSTITUTE(F2,"/","@",LEN(F2)-LEN(SUBSTITUTE(F2,"/",""))))))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3409,7 +3488,7 @@
       <selection activeCell="E1" sqref="E1"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
-      <selection pane="bottomRight" activeCell="S149" sqref="S149"/>
+      <selection pane="bottomRight" activeCell="E1" sqref="E1:M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -6388,44 +6467,49 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I1:J98 I156:J1048576">
-    <cfRule type="cellIs" dxfId="17" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="7" operator="equal">
       <formula>"Custom License"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="8" operator="equal">
       <formula>"All Rights Reserved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I101:J155">
-    <cfRule type="cellIs" dxfId="15" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="1" operator="equal">
       <formula>"Custom License"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="2" operator="equal">
       <formula>"All Rights Reserved"</formula>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="M153" r:id="rId1" xr:uid="{0297EA0E-AABC-42E6-BD9C-C92D40E3D114}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7EE4BB5-BB59-4BD4-AC53-F528CD7FAB04}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:I6"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="19.88671875" customWidth="1"/>
     <col min="2" max="2" width="64.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24" customWidth="1"/>
     <col min="8" max="8" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>244</v>
       </c>
@@ -6445,7 +6529,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>443</v>
       </c>
@@ -6456,14 +6540,16 @@
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
+      <c r="G4" s="9" t="s">
+        <v>877</v>
+      </c>
       <c r="H4" s="9"/>
       <c r="I4" s="9" t="str">
         <f>LEFT(B4, FIND("/releases", B4) - 1)</f>
         <v>https://github.com/Jonius7/Electrodynamics</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>575</v>
       </c>
@@ -6483,22 +6569,43 @@
         <v>https://github.com/GTNewHorizons/AE2FluidCraft-Rework</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="16" t="s">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>441</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="16" t="s">
         <v>442</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="17" t="str">
+      <c r="G6" t="s">
+        <v>876</v>
+      </c>
+      <c r="I6" s="16" t="str">
         <f>LEFT(B6, FIND("/releases", B6) - 1)</f>
         <v>https://github.com/age-series/ElectricalAge</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="18" t="s">
+        <v>576</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>577</v>
+      </c>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18" t="s">
+        <v>875</v>
+      </c>
+      <c r="H7" s="18"/>
+      <c r="I7" s="10" t="str">
+        <f>LEFT(B7, FIND("/releases", B7) - 1)</f>
+        <v>https://github.com/GTNewHorizons/Nuclear-Control</v>
+      </c>
+      <c r="J7" s="18" t="str">
+        <f>IF(D7&lt;&gt;"", D7, RIGHT(B7,LEN(B7)-FIND("@",SUBSTITUTE(B7,"/","@",LEN(B7)-LEN(SUBSTITUTE(B7,"/",""))))))</f>
+        <v>IC2NuclearControl-2.6.19.jar</v>
       </c>
     </row>
   </sheetData>
@@ -6518,9 +6625,9 @@
   <dimension ref="A1:O119"/>
   <sheetViews>
     <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="E33" sqref="E33"/>
+      <selection pane="bottomLeft" activeCell="E115" sqref="E115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -7654,7 +7761,7 @@
         <v>276</v>
       </c>
       <c r="M62" s="4" t="e">
-        <f>LEFT(F62, FIND("/releases", F62) - 1)</f>
+        <f t="shared" ref="M62:M93" si="4">LEFT(F62, FIND("/releases", F62) - 1)</f>
         <v>#VALUE!</v>
       </c>
       <c r="N62" t="str">
@@ -7673,7 +7780,7 @@
         <v>302</v>
       </c>
       <c r="M63" s="4" t="str">
-        <f>LEFT(F63, FIND("/releases", F63) - 1)</f>
+        <f t="shared" si="4"/>
         <v>https://github.com/Jonius7/FullThrottleAlchemistFix</v>
       </c>
       <c r="N63" t="str">
@@ -7692,7 +7799,7 @@
         <v>363</v>
       </c>
       <c r="M64" s="4" t="e">
-        <f>LEFT(F64, FIND("/releases", F64) - 1)</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
       <c r="N64" t="str">
@@ -7708,7 +7815,7 @@
         <v>349</v>
       </c>
       <c r="M65" s="4" t="str">
-        <f>LEFT(F65, FIND("/releases", F65) - 1)</f>
+        <f t="shared" si="4"/>
         <v>https://github.com/GTNewHorizons/EnderIO</v>
       </c>
       <c r="N65" t="str">
@@ -7724,11 +7831,11 @@
         <v>352</v>
       </c>
       <c r="M66" s="4" t="e">
-        <f>LEFT(F66, FIND("/releases", F66) - 1)</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
       <c r="N66" t="str">
-        <f t="shared" ref="N66:N97" si="4">IF(H66&lt;&gt;"", H66, RIGHT(F66,LEN(F66)-FIND("@",SUBSTITUTE(F66,"/","@",LEN(F66)-LEN(SUBSTITUTE(F66,"/",""))))))</f>
+        <f t="shared" ref="N66:N97" si="5">IF(H66&lt;&gt;"", H66, RIGHT(F66,LEN(F66)-FIND("@",SUBSTITUTE(F66,"/","@",LEN(F66)-LEN(SUBSTITUTE(F66,"/",""))))))</f>
         <v>TooManyDanyOres-1.7.10-b1.0-3-forge-1199.jar</v>
       </c>
     </row>
@@ -7743,11 +7850,11 @@
         <v>276</v>
       </c>
       <c r="M67" s="4" t="e">
-        <f>LEFT(F67, FIND("/releases", F67) - 1)</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
       <c r="N67" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>advancedgenetics-1.7.10-1.5.9.jar</v>
       </c>
     </row>
@@ -7762,11 +7869,11 @@
         <v>276</v>
       </c>
       <c r="M68" s="4" t="e">
-        <f>LEFT(F68, FIND("/releases", F68) - 1)</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
       <c r="N68" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>adv-repulsion-systems-59.0.4.jar</v>
       </c>
     </row>
@@ -7781,11 +7888,11 @@
         <v>366</v>
       </c>
       <c r="M69" s="4" t="e">
-        <f>LEFT(F69, FIND("/releases", F69) - 1)</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
       <c r="N69" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>AdvancedSolarPanel-1.7.10-3.5.1.jar</v>
       </c>
     </row>
@@ -7797,11 +7904,11 @@
         <v>368</v>
       </c>
       <c r="M70" s="4" t="str">
-        <f>LEFT(F70, FIND("/releases", F70) - 1)</f>
+        <f t="shared" si="4"/>
         <v>https://github.com/GTNewHorizons/ae2stuff</v>
       </c>
       <c r="N70" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>ae2stuff-0.9.7-GTNH.jar</v>
       </c>
     </row>
@@ -7813,11 +7920,11 @@
         <v>375</v>
       </c>
       <c r="M71" s="4" t="e">
-        <f>LEFT(F71, FIND("/releases", F71) - 1)</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
       <c r="N71" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>AOBD-2.9.2.jar</v>
       </c>
     </row>
@@ -7829,11 +7936,11 @@
         <v>376</v>
       </c>
       <c r="M72" s="4" t="e">
-        <f>LEFT(F72, FIND("/releases", F72) - 1)</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
       <c r="N72" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>AOBDBB-1.0.6.jar</v>
       </c>
     </row>
@@ -7851,11 +7958,11 @@
         <v>277</v>
       </c>
       <c r="M73" s="4" t="str">
-        <f>LEFT(F73, FIND("/releases", F73) - 1)</f>
+        <f t="shared" si="4"/>
         <v>https://github.com/GTNewHorizons/AntiqueAtlas</v>
       </c>
       <c r="N73" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>antiqueatlas-4.4.6-GTNH.jar</v>
       </c>
     </row>
@@ -7867,11 +7974,11 @@
         <v>379</v>
       </c>
       <c r="M74" s="4" t="str">
-        <f>LEFT(F74, FIND("/releases", F74) - 1)</f>
+        <f t="shared" si="4"/>
         <v>https://github.com/GTNewHorizons/WirelessCraftingTerminal</v>
       </c>
       <c r="N74" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>WirelessCraftingTerminal-1.12.7.jar</v>
       </c>
     </row>
@@ -7886,11 +7993,11 @@
         <v>283</v>
       </c>
       <c r="M75" s="4" t="str">
-        <f>LEFT(F75, FIND("/releases", F75) - 1)</f>
+        <f t="shared" si="4"/>
         <v>https://github.com/GTNewHorizons/ArchitectureCraft</v>
       </c>
       <c r="N75" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>ArchitectureCraft-1.11.4.jar</v>
       </c>
     </row>
@@ -7905,11 +8012,11 @@
         <v>283</v>
       </c>
       <c r="M76" s="4" t="str">
-        <f>LEFT(F76, FIND("/releases", F76) - 1)</f>
+        <f t="shared" si="4"/>
         <v>https://github.com/GTNewHorizons/Computronics</v>
       </c>
       <c r="N76" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Computronics-1.9.3-GTNH.jar</v>
       </c>
     </row>
@@ -7924,11 +8031,11 @@
         <v>302</v>
       </c>
       <c r="M77" s="4" t="str">
-        <f>LEFT(F77, FIND("/releases", F77) - 1)</f>
+        <f t="shared" si="4"/>
         <v>https://github.com/GTNewHorizons/Minecraft-Backpack-Mod</v>
       </c>
       <c r="N77" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>backpack-2.5.6-GTNH.jar</v>
       </c>
     </row>
@@ -7943,11 +8050,11 @@
         <v>283</v>
       </c>
       <c r="M78" s="4" t="str">
-        <f>LEFT(F78, FIND("/releases", F78) - 1)</f>
+        <f t="shared" si="4"/>
         <v>https://github.com/copygirl/BetterStorage</v>
       </c>
       <c r="N78" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>BetterStorage-1.7.10-0.13.1.128.jar</v>
       </c>
     </row>
@@ -7959,11 +8066,11 @@
         <v>408</v>
       </c>
       <c r="M79" s="4" t="str">
-        <f>LEFT(F79, FIND("/releases", F79) - 1)</f>
+        <f t="shared" si="4"/>
         <v>https://github.com/GTNewHorizons/BeeBetterAtBees-GTNH</v>
       </c>
       <c r="N79" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>beebetteratbees-0.4.3-GTNH.jar</v>
       </c>
     </row>
@@ -7978,11 +8085,11 @@
         <v>426</v>
       </c>
       <c r="M80" s="4" t="str">
-        <f>LEFT(F80, FIND("/releases", F80) - 1)</f>
+        <f t="shared" si="4"/>
         <v>https://github.com/GTNewHorizons/CarpentersBlocks</v>
       </c>
       <c r="N80" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>CarpentersBlocks-3.7.0-GTNH.jar</v>
       </c>
     </row>
@@ -7997,11 +8104,11 @@
         <v>431</v>
       </c>
       <c r="M81" s="4" t="str">
-        <f>LEFT(F81, FIND("/releases", F81) - 1)</f>
+        <f t="shared" si="4"/>
         <v>https://github.com/GTNewHorizons/CookingForBlockheads</v>
       </c>
       <c r="N81" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>CookingForBlockheads-1.4.4-GTNH.jar</v>
       </c>
     </row>
@@ -8013,11 +8120,11 @@
         <v>435</v>
       </c>
       <c r="M82" s="4" t="str">
-        <f>LEFT(F82, FIND("/releases", F82) - 1)</f>
+        <f t="shared" si="4"/>
         <v>https://github.com/GTNewHorizons/CraftingTweaks</v>
       </c>
       <c r="N82" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>craftingtweaks-1.1.0-GTNH.jar</v>
       </c>
     </row>
@@ -8029,11 +8136,11 @@
         <v>438</v>
       </c>
       <c r="M83" s="4" t="e">
-        <f>LEFT(F83, FIND("/releases", F83) - 1)</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
       <c r="N83" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>cogs-1.7.10-0.1.4.jar</v>
       </c>
     </row>
@@ -8045,11 +8152,11 @@
         <v>178</v>
       </c>
       <c r="M84" s="4" t="str">
-        <f>LEFT(F84, FIND("/releases", F84) - 1)</f>
+        <f t="shared" si="4"/>
         <v>https://github.com/GTNewHorizons/Draconic-Evolution</v>
       </c>
       <c r="N84" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Draconic-Evolution-1.4.24-GTNH.jar</v>
       </c>
     </row>
@@ -8064,11 +8171,11 @@
         <v>255</v>
       </c>
       <c r="M85" s="4" t="str">
-        <f>LEFT(F85, FIND("/releases", F85) - 1)</f>
+        <f t="shared" si="4"/>
         <v>https://github.com/Jonius7/ElectricalAge</v>
       </c>
       <c r="N85" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Eln-1.22.4.jar</v>
       </c>
     </row>
@@ -8083,11 +8190,11 @@
         <v>283</v>
       </c>
       <c r="M86" s="4" t="str">
-        <f>LEFT(F86, FIND("/releases", F86) - 1)</f>
+        <f t="shared" si="4"/>
         <v>https://github.com/GTNewHorizons/EnderStorage</v>
       </c>
       <c r="N86" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>EnderStorage-1.7.7.jar</v>
       </c>
     </row>
@@ -8102,11 +8209,11 @@
         <v>283</v>
       </c>
       <c r="M87" s="4" t="str">
-        <f>LEFT(F87, FIND("/releases", F87) - 1)</f>
+        <f t="shared" si="4"/>
         <v>https://github.com/GTNewHorizons/ExtraCells2</v>
       </c>
       <c r="N87" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>ExtraCells-2.5.35.jar</v>
       </c>
     </row>
@@ -8118,11 +8225,11 @@
         <v>460</v>
       </c>
       <c r="M88" s="4" t="str">
-        <f>LEFT(F88, FIND("/releases", F88) - 1)</f>
+        <f t="shared" si="4"/>
         <v>https://github.com/GTNewHorizons/ForbiddenMagic</v>
       </c>
       <c r="N88" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Forbidden.Magic-0.8.3-GTNH.jar</v>
       </c>
     </row>
@@ -8134,11 +8241,11 @@
         <v>462</v>
       </c>
       <c r="M89" s="4" t="str">
-        <f>LEFT(F89, FIND("/releases", F89) - 1)</f>
+        <f t="shared" si="4"/>
         <v>https://github.com/GTNewHorizons/ForgeRelocationFMP</v>
       </c>
       <c r="N89" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>ForgeRelocationFMP-0.2.0.jar</v>
       </c>
     </row>
@@ -8153,11 +8260,11 @@
         <v>302</v>
       </c>
       <c r="M90" s="4" t="str">
-        <f>LEFT(F90, FIND("/releases", F90) - 1)</f>
+        <f t="shared" si="4"/>
         <v>https://github.com/GTNewHorizons/Gadomancy</v>
       </c>
       <c r="N90" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>gadomancy-1.4.7.jar</v>
       </c>
     </row>
@@ -8169,11 +8276,11 @@
         <v>474</v>
       </c>
       <c r="M91" s="4" t="e">
-        <f>LEFT(F91, FIND("/releases", F91) - 1)</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
       <c r="N91" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>immibis-macroblocks-59.1.1.jar</v>
       </c>
     </row>
@@ -8185,11 +8292,11 @@
         <v>476</v>
       </c>
       <c r="M92" s="4" t="e">
-        <f>LEFT(F92, FIND("/releases", F92) - 1)</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
       <c r="N92" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>immibis-peripherals-59.0.3.jar</v>
       </c>
     </row>
@@ -8201,11 +8308,11 @@
         <v>478</v>
       </c>
       <c r="M93" s="4" t="e">
-        <f>LEFT(F93, FIND("/releases", F93) - 1)</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
       <c r="N93" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>infinitubes-59.0.5.jar</v>
       </c>
     </row>
@@ -8217,11 +8324,11 @@
         <v>480</v>
       </c>
       <c r="M94" s="4" t="e">
-        <f t="shared" ref="M94:M118" si="5">LEFT(F94, FIND("/releases", F94) - 1)</f>
+        <f>LEFT(F94, FIND("/releases", F94) - 1)</f>
         <v>#VALUE!</v>
       </c>
       <c r="N94" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>liquid-xp-59.0.2.jar</v>
       </c>
     </row>
@@ -8236,11 +8343,11 @@
         <v>250</v>
       </c>
       <c r="M95" s="4" t="e">
+        <f>LEFT(F95, FIND("/releases", F95) - 1)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N95" t="str">
         <f t="shared" si="5"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N95" t="str">
-        <f t="shared" si="4"/>
         <v>IGW-Mod-1.7.10-1.1.12-34-universal.jar</v>
       </c>
     </row>
@@ -8255,11 +8362,11 @@
         <v>488</v>
       </c>
       <c r="M96" s="4" t="str">
+        <f>LEFT(F96, FIND("/releases", F96) - 1)</f>
+        <v>https://github.com/GTNewHorizons/LogisticsPipes</v>
+      </c>
+      <c r="N96" t="str">
         <f t="shared" si="5"/>
-        <v>https://github.com/GTNewHorizons/LogisticsPipes</v>
-      </c>
-      <c r="N96" t="str">
-        <f t="shared" si="4"/>
         <v>logisticspipes-1.4.23-GTNH-pre.jar</v>
       </c>
     </row>
@@ -8271,11 +8378,11 @@
         <v>508</v>
       </c>
       <c r="M97" s="4" t="e">
+        <f>LEFT(F97, FIND("/releases", F97) - 1)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N97" t="str">
         <f t="shared" si="5"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N97" t="str">
-        <f t="shared" si="4"/>
         <v>PneumaticCompressing-1.0.5.jar</v>
       </c>
     </row>
@@ -8287,11 +8394,11 @@
         <v>210</v>
       </c>
       <c r="M98" s="4" t="e">
-        <f t="shared" si="5"/>
+        <f>LEFT(F98, FIND("/releases", F98) - 1)</f>
         <v>#VALUE!</v>
       </c>
       <c r="N98" t="str">
-        <f t="shared" ref="N98:N119" si="6">IF(H98&lt;&gt;"", H98, RIGHT(F98,LEN(F98)-FIND("@",SUBSTITUTE(F98,"/","@",LEN(F98)-LEN(SUBSTITUTE(F98,"/",""))))))</f>
+        <f>IF(H98&lt;&gt;"", H98, RIGHT(F98,LEN(F98)-FIND("@",SUBSTITUTE(F98,"/","@",LEN(F98)-LEN(SUBSTITUTE(F98,"/",""))))))</f>
         <v>SolarExpansion-Basic-1.6a.jar</v>
       </c>
     </row>
@@ -8306,11 +8413,11 @@
         <v>277</v>
       </c>
       <c r="M99" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f>LEFT(F99, FIND("/releases", F99) - 1)</f>
         <v>https://github.com/GTNewHorizons/ThaumicEnergistics</v>
       </c>
       <c r="N99" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(H99&lt;&gt;"", H99, RIGHT(F99,LEN(F99)-FIND("@",SUBSTITUTE(F99,"/","@",LEN(F99)-LEN(SUBSTITUTE(F99,"/",""))))))</f>
         <v>thaumicenergistics-1.7.11-GTNH.jar</v>
       </c>
     </row>
@@ -8325,11 +8432,11 @@
         <v>516</v>
       </c>
       <c r="M100" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f>LEFT(F100, FIND("/releases", F100) - 1)</f>
         <v>https://github.com/GTNewHorizons/Thaumic_Exploration</v>
       </c>
       <c r="N100" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(H100&lt;&gt;"", H100, RIGHT(F100,LEN(F100)-FIND("@",SUBSTITUTE(F100,"/","@",LEN(F100)-LEN(SUBSTITUTE(F100,"/",""))))))</f>
         <v>Thaumic-Exploration-1.4.6-GTNH-pre.jar</v>
       </c>
     </row>
@@ -8344,11 +8451,11 @@
         <v>523</v>
       </c>
       <c r="M101" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f>LEFT(F101, FIND("/releases", F101) - 1)</f>
         <v>https://github.com/GTNewHorizons/ThaumicTinkerer</v>
       </c>
       <c r="N101" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(H101&lt;&gt;"", H101, RIGHT(F101,LEN(F101)-FIND("@",SUBSTITUTE(F101,"/","@",LEN(F101)-LEN(SUBSTITUTE(F101,"/",""))))))</f>
         <v>ThaumicTinkerer-2.11.20.jar</v>
       </c>
     </row>
@@ -8363,11 +8470,11 @@
         <v>426</v>
       </c>
       <c r="M102" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f>LEFT(F102, FIND("/releases", F102) - 1)</f>
         <v>https://github.com/GTNewHorizons/twilightforest</v>
       </c>
       <c r="N102" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(H102&lt;&gt;"", H102, RIGHT(F102,LEN(F102)-FIND("@",SUBSTITUTE(F102,"/","@",LEN(F102)-LEN(SUBSTITUTE(F102,"/",""))))))</f>
         <v>TwilightForest-2.7.11.jar</v>
       </c>
     </row>
@@ -8385,11 +8492,11 @@
         <v>531</v>
       </c>
       <c r="M103" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f>LEFT(F103, FIND("/releases", F103) - 1)</f>
         <v>https://github.com/GTNewHorizons/TiC-Tooltips</v>
       </c>
       <c r="N103" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(H103&lt;&gt;"", H103, RIGHT(F103,LEN(F103)-FIND("@",SUBSTITUTE(F103,"/","@",LEN(F103)-LEN(SUBSTITUTE(F103,"/",""))))))</f>
         <v>TiCTooltips-1.4.0.jar</v>
       </c>
     </row>
@@ -8404,11 +8511,11 @@
         <v>283</v>
       </c>
       <c r="M104" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f>LEFT(F104, FIND("/releases", F104) - 1)</f>
         <v>https://github.com/GTNewHorizons/TinkersMechworks</v>
       </c>
       <c r="N104" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(H104&lt;&gt;"", H104, RIGHT(F104,LEN(F104)-FIND("@",SUBSTITUTE(F104,"/","@",LEN(F104)-LEN(SUBSTITUTE(F104,"/",""))))))</f>
         <v>TMechworks-0.4.1.jar</v>
       </c>
     </row>
@@ -8420,11 +8527,11 @@
         <v>540</v>
       </c>
       <c r="M105" s="4" t="e">
-        <f t="shared" si="5"/>
+        <f>LEFT(F105, FIND("/releases", F105) - 1)</f>
         <v>#VALUE!</v>
       </c>
       <c r="N105" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(H105&lt;&gt;"", H105, RIGHT(F105,LEN(F105)-FIND("@",SUBSTITUTE(F105,"/","@",LEN(F105)-LEN(SUBSTITUTE(F105,"/",""))))))</f>
         <v>tubestuff-59.0.4.jar</v>
       </c>
     </row>
@@ -8436,11 +8543,11 @@
         <v>544</v>
       </c>
       <c r="M106" s="4" t="e">
-        <f t="shared" si="5"/>
+        <f>LEFT(F106, FIND("/releases", F106) - 1)</f>
         <v>#VALUE!</v>
       </c>
       <c r="N106" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(H106&lt;&gt;"", H106, RIGHT(F106,LEN(F106)-FIND("@",SUBSTITUTE(F106,"/","@",LEN(F106)-LEN(SUBSTITUTE(F106,"/",""))))))</f>
         <v>UniverseCraft-1.7.10-V1.4.2.jar</v>
       </c>
     </row>
@@ -8452,11 +8559,11 @@
         <v>553</v>
       </c>
       <c r="M107" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f>LEFT(F107, FIND("/releases", F107) - 1)</f>
         <v>https://github.com/GTNewHorizons/gendustry</v>
       </c>
       <c r="N107" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(H107&lt;&gt;"", H107, RIGHT(F107,LEN(F107)-FIND("@",SUBSTITUTE(F107,"/","@",LEN(F107)-LEN(SUBSTITUTE(F107,"/",""))))))</f>
         <v>gendustry-1.9.4-GTNH.jar</v>
       </c>
     </row>
@@ -8468,11 +8575,11 @@
         <v>559</v>
       </c>
       <c r="M108" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f>LEFT(F108, FIND("/releases", F108) - 1)</f>
         <v>https://github.com/Jonius7/EnderIOAddons</v>
       </c>
       <c r="N108" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(H108&lt;&gt;"", H108, RIGHT(F108,LEN(F108)-FIND("@",SUBSTITUTE(F108,"/","@",LEN(F108)-LEN(SUBSTITUTE(F108,"/",""))))))</f>
         <v>enderioaddons-1.7.10-0.10.16.jar</v>
       </c>
     </row>
@@ -8490,11 +8597,11 @@
         <v>563</v>
       </c>
       <c r="M109" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f>LEFT(F109, FIND("/releases", F109) - 1)</f>
         <v>https://github.com/GTNewHorizons/AkashicTome</v>
       </c>
       <c r="N109" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(H109&lt;&gt;"", H109, RIGHT(F109,LEN(F109)-FIND("@",SUBSTITUTE(F109,"/","@",LEN(F109)-LEN(SUBSTITUTE(F109,"/",""))))))</f>
         <v>akashictome-1.2.6.jar</v>
       </c>
     </row>
@@ -8512,11 +8619,11 @@
         <v>283</v>
       </c>
       <c r="M110" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f>LEFT(F110, FIND("/releases", F110) - 1)</f>
         <v>https://github.com/idkidknow/IE1710NEIPatch</v>
       </c>
       <c r="N110" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(H110&lt;&gt;"", H110, RIGHT(F110,LEN(F110)-FIND("@",SUBSTITUTE(F110,"/","@",LEN(F110)-LEN(SUBSTITUTE(F110,"/",""))))))</f>
         <v>ie1710neipatch-0.1.1.jar</v>
       </c>
     </row>
@@ -8528,165 +8635,169 @@
         <v>572</v>
       </c>
       <c r="M111" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f>LEFT(F111, FIND("/releases", F111) - 1)</f>
         <v>https://github.com/GTNewHorizons/FTB-Utilities</v>
       </c>
       <c r="N111" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(H111&lt;&gt;"", H111, RIGHT(F111,LEN(F111)-FIND("@",SUBSTITUTE(F111,"/","@",LEN(F111)-LEN(SUBSTITUTE(F111,"/",""))))))</f>
         <v>FTBUtilities-1.1.1-GTNH.jar</v>
       </c>
     </row>
     <row r="112" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E112" t="s">
-        <v>576</v>
+        <v>579</v>
       </c>
       <c r="F112" s="4" t="s">
-        <v>577</v>
+        <v>578</v>
+      </c>
+      <c r="J112" t="s">
+        <v>254</v>
       </c>
       <c r="M112" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>https://github.com/GTNewHorizons/Nuclear-Control</v>
+        <f>LEFT(F112, FIND("/releases", F112) - 1)</f>
+        <v>https://github.com/GTNewHorizons/ProjectBlue</v>
       </c>
       <c r="N112" t="str">
-        <f t="shared" si="6"/>
-        <v>IC2NuclearControl-2.6.19.jar</v>
+        <f>IF(H112&lt;&gt;"", H112, RIGHT(F112,LEN(F112)-FIND("@",SUBSTITUTE(F112,"/","@",LEN(F112)-LEN(SUBSTITUTE(F112,"/",""))))))</f>
+        <v>ProjectBlue-1.2.0-GTNH.jar</v>
       </c>
     </row>
     <row r="113" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E113" t="s">
-        <v>579</v>
+        <v>582</v>
       </c>
       <c r="F113" s="4" t="s">
-        <v>578</v>
+        <v>583</v>
       </c>
       <c r="J113" t="s">
-        <v>254</v>
+        <v>283</v>
       </c>
       <c r="M113" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>https://github.com/GTNewHorizons/ProjectBlue</v>
+        <f>LEFT(F113, FIND("/releases", F113) - 1)</f>
+        <v>https://github.com/GTNewHorizons/WirelessRedstone-CBE</v>
       </c>
       <c r="N113" t="str">
-        <f t="shared" si="6"/>
-        <v>ProjectBlue-1.2.0-GTNH.jar</v>
+        <f>IF(H113&lt;&gt;"", H113, RIGHT(F113,LEN(F113)-FIND("@",SUBSTITUTE(F113,"/","@",LEN(F113)-LEN(SUBSTITUTE(F113,"/",""))))))</f>
+        <v>WR-CBE-1.7.1.jar</v>
       </c>
     </row>
     <row r="114" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E114" t="s">
-        <v>582</v>
-      </c>
-      <c r="F114" s="4" t="s">
-        <v>583</v>
+        <v>49</v>
+      </c>
+      <c r="F114" s="11" t="s">
+        <v>50</v>
       </c>
       <c r="J114" t="s">
-        <v>283</v>
+        <v>297</v>
       </c>
       <c r="M114" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>https://github.com/GTNewHorizons/WirelessRedstone-CBE</v>
+        <f>LEFT(F114, FIND("/releases", F114) - 1)</f>
+        <v>https://github.com/GTNewHorizons/Chisel</v>
       </c>
       <c r="N114" t="str">
-        <f t="shared" si="6"/>
-        <v>WR-CBE-1.7.1.jar</v>
+        <f>IF(H114&lt;&gt;"", H114, RIGHT(F114,LEN(F114)-FIND("@",SUBSTITUTE(F114,"/","@",LEN(F114)-LEN(SUBSTITUTE(F114,"/",""))))))</f>
+        <v>chisel-2.16.11-GTNH.jar</v>
       </c>
     </row>
     <row r="115" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E115" t="s">
-        <v>49</v>
-      </c>
-      <c r="F115" s="11" t="s">
-        <v>50</v>
+        <v>414</v>
+      </c>
+      <c r="F115" s="4" t="s">
+        <v>590</v>
       </c>
       <c r="J115" t="s">
-        <v>297</v>
+        <v>591</v>
       </c>
       <c r="M115" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>https://github.com/GTNewHorizons/Chisel</v>
+        <f>LEFT(F115, FIND("/releases", F115) - 1)</f>
+        <v>https://github.com/DrParadox7/Binnie</v>
       </c>
       <c r="N115" t="str">
-        <f t="shared" si="6"/>
-        <v>chisel-2.16.11-GTNH.jar</v>
+        <f>IF(H115&lt;&gt;"", H115, RIGHT(F115,LEN(F115)-FIND("@",SUBSTITUTE(F115,"/","@",LEN(F115)-LEN(SUBSTITUTE(F115,"/",""))))))</f>
+        <v>binnie-mods-v2.1.15-LE.jar</v>
       </c>
     </row>
     <row r="116" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E116" t="s">
-        <v>414</v>
+        <v>165</v>
       </c>
       <c r="F116" s="4" t="s">
-        <v>590</v>
+        <v>639</v>
       </c>
       <c r="J116" t="s">
-        <v>591</v>
+        <v>283</v>
       </c>
       <c r="M116" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>https://github.com/DrParadox7/Binnie</v>
+        <f>LEFT(F116, FIND("/releases", F116) - 1)</f>
+        <v>https://github.com/Jonius7/NuclearCraft</v>
       </c>
       <c r="N116" t="str">
-        <f t="shared" si="6"/>
-        <v>binnie-mods-v2.1.15-LE.jar</v>
+        <f>IF(H116&lt;&gt;"", H116, RIGHT(F116,LEN(F116)-FIND("@",SUBSTITUTE(F116,"/","@",LEN(F116)-LEN(SUBSTITUTE(F116,"/",""))))))</f>
+        <v>NuclearCraft-1.9h--1.7.10.jar</v>
       </c>
     </row>
     <row r="117" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E117" t="s">
-        <v>165</v>
+        <v>564</v>
       </c>
       <c r="F117" s="4" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="J117" t="s">
         <v>283</v>
       </c>
       <c r="M117" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>https://github.com/Jonius7/NuclearCraft</v>
+        <f>LEFT(F117, FIND("/releases", F117) - 1)</f>
+        <v>https://github.com/GTNewHorizons/BetterQuesting</v>
       </c>
       <c r="N117" t="str">
-        <f t="shared" si="6"/>
-        <v>NuclearCraft-1.9h--1.7.10.jar</v>
+        <f>IF(H117&lt;&gt;"", H117, RIGHT(F117,LEN(F117)-FIND("@",SUBSTITUTE(F117,"/","@",LEN(F117)-LEN(SUBSTITUTE(F117,"/",""))))))</f>
+        <v>BetterQuesting-3.7.13-GTNH.jar</v>
       </c>
     </row>
     <row r="118" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E118" t="s">
-        <v>564</v>
+        <v>684</v>
       </c>
       <c r="F118" s="4" t="s">
-        <v>640</v>
-      </c>
-      <c r="J118" t="s">
-        <v>283</v>
-      </c>
-      <c r="M118" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>https://github.com/GTNewHorizons/BetterQuesting</v>
+        <v>685</v>
+      </c>
+      <c r="H118" t="s">
+        <v>686</v>
+      </c>
+      <c r="M118" s="4" t="e">
+        <f>LEFT(F118, FIND("/releases", F118) - 1)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="N118" t="str">
-        <f t="shared" si="6"/>
-        <v>BetterQuesting-3.7.13-GTNH.jar</v>
+        <f>IF(H118&lt;&gt;"", H118, RIGHT(F118,LEN(F118)-FIND("@",SUBSTITUTE(F118,"/","@",LEN(F118)-LEN(SUBSTITUTE(F118,"/",""))))))</f>
+        <v>ztech1.7.10-0.0.3.jar</v>
       </c>
     </row>
     <row r="119" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E119" t="s">
-        <v>684</v>
-      </c>
-      <c r="F119" s="18" t="s">
-        <v>685</v>
-      </c>
-      <c r="H119" t="s">
-        <v>686</v>
+        <v>873</v>
+      </c>
+      <c r="F119" s="4" t="s">
+        <v>874</v>
+      </c>
+      <c r="M119" s="4" t="e">
+        <f>LEFT(F119, FIND("/releases", F119) - 1)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="N119" t="str">
-        <f t="shared" si="6"/>
-        <v>ztech1.7.10-0.0.3.jar</v>
+        <f>IF(H119&lt;&gt;"", H119, RIGHT(F119,LEN(F119)-FIND("@",SUBSTITUTE(F119,"/","@",LEN(F119)-LEN(SUBSTITUTE(F119,"/",""))))))</f>
+        <v>Technomancy - 0.12.5 - 1.7.10.jar</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="J3">
-    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="1" operator="equal">
       <formula>"Custom License"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
       <formula>"All Rights Reserved"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8715,7 +8826,7 @@
     <hyperlink ref="F64" r:id="rId22" xr:uid="{B8FCB286-55CA-4FE1-8CFF-848571A49E35}"/>
     <hyperlink ref="F87" r:id="rId23" xr:uid="{2F3C44CC-DFFC-46FB-9766-C7ADEE788EF2}"/>
     <hyperlink ref="F88" r:id="rId24" xr:uid="{8A99A28C-926F-43C4-9589-8C3F8FAC6152}"/>
-    <hyperlink ref="F115" r:id="rId25" xr:uid="{19D106F6-F7E3-4EF4-A31C-E0C73E00BE2B}"/>
+    <hyperlink ref="F114" r:id="rId25" xr:uid="{19D106F6-F7E3-4EF4-A31C-E0C73E00BE2B}"/>
     <hyperlink ref="F21" r:id="rId26" xr:uid="{86858A87-D198-4358-A164-E46924D9BC89}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8821,12 +8932,12 @@
   </sheetPr>
   <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F14" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="5" ySplit="1" topLeftCell="F11" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
-      <selection pane="bottomRight" activeCell="L26" sqref="L26"/>
+      <selection pane="bottomRight" activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -9427,11 +9538,11 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="I1:I28 I30:I1048576">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
+  <conditionalFormatting sqref="I1:I1048576">
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
       <formula>"Custom License"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
       <formula>"All Rights Reserved"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9451,7 +9562,7 @@
   <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="N15" sqref="N15"/>
     </sheetView>
@@ -9519,7 +9630,7 @@
       <c r="F2" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="M2" s="19" t="str">
+      <c r="M2" s="17" t="str">
         <f t="shared" ref="M2:M12" si="0">LEFT(F2, FIND("/releases", F2) - 1)</f>
         <v>https://github.com/Jonius7/Mantle</v>
       </c>
@@ -9535,7 +9646,7 @@
       <c r="F3" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="M3" s="19" t="str">
+      <c r="M3" s="17" t="str">
         <f t="shared" si="0"/>
         <v>https://github.com/GTNewHorizons/EnderCore</v>
       </c>
@@ -9551,7 +9662,7 @@
       <c r="F4" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="M4" s="19" t="str">
+      <c r="M4" s="17" t="str">
         <f t="shared" si="0"/>
         <v>https://github.com/GTNewHorizons/OpenModsLib</v>
       </c>
@@ -9567,7 +9678,7 @@
       <c r="F5" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="M5" s="19" t="str">
+      <c r="M5" s="17" t="str">
         <f t="shared" si="0"/>
         <v>https://github.com/GTNewHorizons/MrTJPCore</v>
       </c>
@@ -9583,7 +9694,7 @@
       <c r="F6" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="M6" s="19" t="str">
+      <c r="M6" s="17" t="str">
         <f t="shared" si="0"/>
         <v>https://github.com/GTNewHorizons/BrandonsCore</v>
       </c>
@@ -9599,7 +9710,7 @@
       <c r="F7" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="M7" s="19" t="str">
+      <c r="M7" s="17" t="str">
         <f t="shared" si="0"/>
         <v>https://github.com/GTNewHorizons/LunatriusCore</v>
       </c>
@@ -9615,7 +9726,7 @@
       <c r="F8" s="4" t="s">
         <v>362</v>
       </c>
-      <c r="M8" s="19" t="e">
+      <c r="M8" s="17" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
@@ -9634,7 +9745,7 @@
       <c r="J9" t="s">
         <v>257</v>
       </c>
-      <c r="M9" s="19" t="str">
+      <c r="M9" s="17" t="str">
         <f t="shared" si="0"/>
         <v>https://github.com/GTNewHorizons/AsieLib</v>
       </c>
@@ -9653,7 +9764,7 @@
       <c r="J10" t="s">
         <v>417</v>
       </c>
-      <c r="M10" s="19" t="str">
+      <c r="M10" s="17" t="str">
         <f t="shared" si="0"/>
         <v>https://github.com/GTNewHorizons/bdlib</v>
       </c>
@@ -9669,7 +9780,7 @@
       <c r="F11" s="4" t="s">
         <v>557</v>
       </c>
-      <c r="M11" s="19" t="str">
+      <c r="M11" s="17" t="str">
         <f t="shared" si="0"/>
         <v>https://github.com/GTNewHorizons/ModularUI2</v>
       </c>
@@ -9685,7 +9796,7 @@
       <c r="F12" s="4" t="s">
         <v>573</v>
       </c>
-      <c r="M12" s="19" t="str">
+      <c r="M12" s="17" t="str">
         <f t="shared" si="0"/>
         <v>https://github.com/GTNewHorizons/FTB-Library</v>
       </c>
@@ -9711,7 +9822,7 @@
       <c r="L13" s="9" t="s">
         <v>289</v>
       </c>
-      <c r="M13" s="19" t="str">
+      <c r="M13" s="17" t="str">
         <f>LEFT(F13, FIND("/releases", F13) - 1)</f>
         <v>https://github.com/GTNewHorizons/ForgeMultipart</v>
       </c>
@@ -9913,7 +10024,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10083,9 +10194,15 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C13" s="4" t="e">
+      <c r="A13">
+        <v>2295819</v>
+      </c>
+      <c r="B13" t="s">
+        <v>872</v>
+      </c>
+      <c r="C13" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v>https://mediafilez.forgecdn.net/files/2295/819/Technomancy - 0.12.5 - 1.7.10.jar</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -10110,21 +10227,22 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E8BB584-5680-4F0E-93DA-8135C8293787}">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.88671875" customWidth="1"/>
     <col min="2" max="2" width="32.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5546875" customWidth="1"/>
-    <col min="4" max="4" width="18.77734375" customWidth="1"/>
+    <col min="4" max="4" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>356</v>
       </c>
@@ -10138,7 +10256,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>280</v>
       </c>
@@ -10152,7 +10270,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>469</v>
       </c>
@@ -10169,7 +10287,36 @@
         <v>470</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="19" t="s">
+        <v>244</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>249</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>239</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>288</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>263</v>
+      </c>
+      <c r="H5" s="19" t="s">
+        <v>342</v>
+      </c>
+      <c r="I5" s="19" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>418</v>
       </c>
@@ -10182,8 +10329,11 @@
       <c r="E6" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G6" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>440</v>
       </c>
@@ -10196,8 +10346,11 @@
       <c r="E7" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G7" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>439</v>
       </c>
@@ -10207,8 +10360,11 @@
       <c r="C8">
         <v>2692129</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G8" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>471</v>
       </c>
@@ -10221,8 +10377,11 @@
       <c r="E9" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G9" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>472</v>
       </c>
@@ -10235,8 +10394,11 @@
       <c r="E10" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G10" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>491</v>
       </c>
@@ -10246,8 +10408,11 @@
       <c r="C11">
         <v>3870763</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G11" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>534</v>
       </c>
@@ -10260,8 +10425,11 @@
       <c r="E12" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G12" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>427</v>
       </c>
@@ -10274,8 +10442,11 @@
       <c r="E13" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G13" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>49</v>
       </c>
@@ -10288,8 +10459,11 @@
       <c r="E14" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G14" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>560</v>
       </c>
@@ -10305,8 +10479,11 @@
       <c r="F15" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G15" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>509</v>
       </c>
@@ -10316,11 +10493,11 @@
       <c r="C16">
         <v>2333989</v>
       </c>
-      <c r="D16" t="s">
-        <v>588</v>
-      </c>
       <c r="E16" t="s">
         <v>241</v>
+      </c>
+      <c r="G16" t="s">
+        <v>588</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
@@ -10336,6 +10513,9 @@
       <c r="E17" t="s">
         <v>255</v>
       </c>
+      <c r="G17" t="s">
+        <v>880</v>
+      </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
@@ -10364,6 +10544,9 @@
       <c r="E19" t="s">
         <v>257</v>
       </c>
+      <c r="G19" t="s">
+        <v>879</v>
+      </c>
       <c r="H19" t="s">
         <v>604</v>
       </c>
@@ -10381,6 +10564,9 @@
       <c r="E20" t="s">
         <v>241</v>
       </c>
+      <c r="G20" t="s">
+        <v>878</v>
+      </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
@@ -10398,6 +10584,9 @@
       <c r="E21" s="9" t="s">
         <v>241</v>
       </c>
+      <c r="G21" t="s">
+        <v>878</v>
+      </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
@@ -10412,6 +10601,9 @@
       <c r="E22" t="s">
         <v>241</v>
       </c>
+      <c r="G22" t="s">
+        <v>878</v>
+      </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
@@ -10423,43 +10615,51 @@
       <c r="C23">
         <v>3030146</v>
       </c>
-      <c r="D23" t="s">
-        <v>588</v>
-      </c>
       <c r="E23" t="s">
         <v>257</v>
       </c>
+      <c r="G23" t="s">
+        <v>588</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E6:E18">
-    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
       <formula>"Custom License"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
       <formula>"All Rights Reserved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E20:E22">
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
       <formula>"Custom License"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="6" operator="equal">
       <formula>"All Rights Reserved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E19:F19">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
       <formula>"Custom License"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
       <formula>"All Rights Reserved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23:F23">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>"Custom License"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+      <formula>"All Rights Reserved"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5:F5">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"Custom License"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"All Rights Reserved"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>